<commit_message>
SAM class 구현 성공
</commit_message>
<xml_diff>
--- a/SAM 양식.xlsx
+++ b/SAM 양식.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongyokim/main/jupyter /2022:Summer/프로젝트/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongyokim/main/jupyter/2022:Summer/프로젝트/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B67A1F6-A3A9-D84F-ACE1-1A45DDE6CE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8F5A43-409F-514B-B8B5-2E04209DFEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{991C2FD3-15E4-3344-A3D5-F7636A9C4AF5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{991C2FD3-15E4-3344-A3D5-F7636A9C4AF5}"/>
   </bookViews>
   <sheets>
     <sheet name="전산업_SAM" sheetId="1" r:id="rId1"/>
     <sheet name="25개 산업_SAM" sheetId="2" r:id="rId2"/>
+    <sheet name="5개 산업_SAM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>산업</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -250,6 +251,14 @@
   </si>
   <si>
     <t>총계</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOC 산업</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공간정보산업</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -894,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EFE132-EA73-A646-9D11-D5672137251A}">
   <dimension ref="A1:AM65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2688,4 +2697,528 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A286B92-10CC-7844-B3F3-3777A9CEC4C5}">
+  <dimension ref="A1:S45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="12"/>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="J20" s="8"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="4"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="J22" s="9"/>
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="B45" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>